<commit_message>
RapportDeveloppement and temps de travail
</commit_message>
<xml_diff>
--- a/tempstravail.xlsx
+++ b/tempstravail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="18915" windowHeight="11820"/>
+    <workbookView xWindow="120" yWindow="72" windowWidth="18912" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,8 +51,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -62,6 +69,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,11 +263,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -263,21 +278,25 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -290,12 +309,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,16 +625,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:I161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F136" sqref="F136"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A217" sqref="A217"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="4" max="5" width="23" customWidth="1"/>
-    <col min="6" max="7" width="22.85546875" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="6" max="7" width="22.88671875" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -633,7 +659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
         <v>42037</v>
       </c>
@@ -656,7 +682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>42038</v>
       </c>
@@ -667,7 +693,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>42039</v>
       </c>
@@ -678,7 +704,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>42040</v>
       </c>
@@ -689,7 +715,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>42041</v>
       </c>
@@ -700,7 +726,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>42042</v>
       </c>
@@ -723,7 +749,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>42043</v>
       </c>
@@ -734,7 +760,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>42044</v>
       </c>
@@ -745,7 +771,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>42045</v>
       </c>
@@ -756,7 +782,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>42046</v>
       </c>
@@ -767,7 +793,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <v>42047</v>
       </c>
@@ -778,7 +804,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
         <v>42048</v>
       </c>
@@ -789,7 +815,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
         <v>42049</v>
       </c>
@@ -800,7 +826,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>42050</v>
       </c>
@@ -811,7 +837,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>42051</v>
       </c>
@@ -822,7 +848,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
         <v>42052</v>
       </c>
@@ -833,7 +859,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
         <v>42053</v>
       </c>
@@ -844,7 +870,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
         <v>42054</v>
       </c>
@@ -867,7 +893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <v>42055</v>
       </c>
@@ -878,7 +904,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
         <v>42056</v>
       </c>
@@ -889,7 +915,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="5">
         <v>42057</v>
       </c>
@@ -900,7 +926,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <v>42058</v>
       </c>
@@ -911,7 +937,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
         <v>42059</v>
       </c>
@@ -922,7 +948,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <v>42060</v>
       </c>
@@ -933,7 +959,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" s="4">
         <v>42061</v>
       </c>
@@ -944,7 +970,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
         <v>42062</v>
       </c>
@@ -955,7 +981,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B32" s="5">
         <v>42063</v>
       </c>
@@ -966,7 +992,7 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B33" s="5">
         <v>42064</v>
       </c>
@@ -977,7 +1003,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B34" s="4">
         <v>42065</v>
       </c>
@@ -988,7 +1014,7 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B35" s="4">
         <v>42066</v>
       </c>
@@ -999,7 +1025,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B36" s="4">
         <v>42067</v>
       </c>
@@ -1010,7 +1036,7 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B37" s="4">
         <v>42068</v>
       </c>
@@ -1033,7 +1059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B38" s="4">
         <v>42069</v>
       </c>
@@ -1044,7 +1070,7 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="5">
         <v>42070</v>
       </c>
@@ -1055,7 +1081,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B40" s="5">
         <v>42071</v>
       </c>
@@ -1066,7 +1092,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B41" s="4">
         <v>42072</v>
       </c>
@@ -1077,7 +1103,7 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B42" s="4">
         <v>42073</v>
       </c>
@@ -1088,7 +1114,7 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B43" s="4">
         <v>42074</v>
       </c>
@@ -1099,7 +1125,7 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B44" s="4">
         <v>42075</v>
       </c>
@@ -1110,7 +1136,7 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B45" s="4">
         <v>42076</v>
       </c>
@@ -1121,7 +1147,7 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B46" s="5">
         <v>42077</v>
       </c>
@@ -1132,7 +1158,7 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B47" s="5">
         <v>42078</v>
       </c>
@@ -1143,7 +1169,7 @@
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B48" s="4">
         <v>42079</v>
       </c>
@@ -1154,7 +1180,7 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B49" s="4">
         <v>42080</v>
       </c>
@@ -1165,7 +1191,7 @@
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B50" s="4">
         <v>42081</v>
       </c>
@@ -1176,7 +1202,7 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B51" s="4">
         <v>42082</v>
       </c>
@@ -1187,7 +1213,7 @@
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B52" s="4">
         <v>42083</v>
       </c>
@@ -1198,7 +1224,7 @@
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B53" s="5">
         <v>42084</v>
       </c>
@@ -1209,7 +1235,7 @@
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B54" s="5">
         <v>42085</v>
       </c>
@@ -1220,7 +1246,7 @@
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B55" s="4">
         <v>42086</v>
       </c>
@@ -1231,7 +1257,7 @@
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B56" s="4">
         <v>42087</v>
       </c>
@@ -1242,7 +1268,7 @@
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B57" s="4">
         <v>42088</v>
       </c>
@@ -1253,7 +1279,7 @@
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B58" s="4">
         <v>42089</v>
       </c>
@@ -1264,7 +1290,7 @@
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B59" s="4">
         <v>42090</v>
       </c>
@@ -1275,7 +1301,7 @@
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B60" s="5">
         <v>42091</v>
       </c>
@@ -1286,7 +1312,7 @@
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B61" s="5">
         <v>42092</v>
       </c>
@@ -1297,7 +1323,7 @@
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B62" s="4">
         <v>42093</v>
       </c>
@@ -1308,7 +1334,7 @@
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B63" s="4">
         <v>42094</v>
       </c>
@@ -1319,7 +1345,7 @@
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B64" s="4">
         <v>42095</v>
       </c>
@@ -1330,7 +1356,7 @@
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B65" s="4">
         <v>42096</v>
       </c>
@@ -1353,7 +1379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B66" s="4">
         <v>42097</v>
       </c>
@@ -1376,7 +1402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B67" s="5">
         <v>42098</v>
       </c>
@@ -1399,7 +1425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B68" s="5">
         <v>42099</v>
       </c>
@@ -1410,7 +1436,7 @@
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B69" s="4">
         <v>42100</v>
       </c>
@@ -1421,7 +1447,7 @@
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B70" s="4">
         <v>42101</v>
       </c>
@@ -1432,7 +1458,7 @@
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B71" s="4">
         <v>42102</v>
       </c>
@@ -1453,7 +1479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B72" s="4">
         <v>42103</v>
       </c>
@@ -1476,7 +1502,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B73" s="4">
         <v>42104</v>
       </c>
@@ -1487,7 +1513,7 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B74" s="5">
         <v>42105</v>
       </c>
@@ -1498,7 +1524,7 @@
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B75" s="5">
         <v>42106</v>
       </c>
@@ -1509,7 +1535,7 @@
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B76" s="4">
         <v>42107</v>
       </c>
@@ -1520,7 +1546,7 @@
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B77" s="4">
         <v>42108</v>
       </c>
@@ -1531,7 +1557,7 @@
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B78" s="4">
         <v>42109</v>
       </c>
@@ -1542,7 +1568,7 @@
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B79" s="4">
         <v>42110</v>
       </c>
@@ -1553,7 +1579,7 @@
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B80" s="4">
         <v>42111</v>
       </c>
@@ -1564,7 +1590,7 @@
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B81" s="5">
         <v>42112</v>
       </c>
@@ -1575,7 +1601,7 @@
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B82" s="5">
         <v>42113</v>
       </c>
@@ -1586,7 +1612,7 @@
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B83" s="4">
         <v>42114</v>
       </c>
@@ -1597,7 +1623,7 @@
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B84" s="4">
         <v>42115</v>
       </c>
@@ -1620,7 +1646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B85" s="4">
         <v>42116</v>
       </c>
@@ -1631,7 +1657,7 @@
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B86" s="4">
         <v>42117</v>
       </c>
@@ -1642,7 +1668,7 @@
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B87" s="4">
         <v>42118</v>
       </c>
@@ -1653,7 +1679,7 @@
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B88" s="5">
         <v>42119</v>
       </c>
@@ -1664,7 +1690,7 @@
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B89" s="5">
         <v>42120</v>
       </c>
@@ -1675,7 +1701,7 @@
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B90" s="4">
         <v>42121</v>
       </c>
@@ -1686,7 +1712,7 @@
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B91" s="4">
         <v>42122</v>
       </c>
@@ -1697,7 +1723,7 @@
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B92" s="4">
         <v>42123</v>
       </c>
@@ -1708,7 +1734,7 @@
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B93" s="4">
         <v>42124</v>
       </c>
@@ -1719,7 +1745,7 @@
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B94" s="4">
         <v>42125</v>
       </c>
@@ -1730,7 +1756,7 @@
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B95" s="5">
         <v>42126</v>
       </c>
@@ -1741,7 +1767,7 @@
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B96" s="5">
         <v>42127</v>
       </c>
@@ -1752,7 +1778,7 @@
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B97" s="4">
         <v>42128</v>
       </c>
@@ -1763,7 +1789,7 @@
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B98" s="4">
         <v>42129</v>
       </c>
@@ -1786,7 +1812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B99" s="4">
         <v>42130</v>
       </c>
@@ -1797,7 +1823,7 @@
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B100" s="4">
         <v>42131</v>
       </c>
@@ -1817,10 +1843,10 @@
         <v>2</v>
       </c>
       <c r="H100" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B101" s="4">
         <v>42132</v>
       </c>
@@ -1831,7 +1857,7 @@
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B102" s="5">
         <v>42133</v>
       </c>
@@ -1854,7 +1880,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B103" s="5">
         <v>42134</v>
       </c>
@@ -1875,7 +1901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B104" s="4">
         <v>42135</v>
       </c>
@@ -1886,7 +1912,7 @@
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B105" s="4">
         <v>42136</v>
       </c>
@@ -1897,7 +1923,7 @@
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B106" s="4">
         <v>42137</v>
       </c>
@@ -1908,7 +1934,7 @@
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B107" s="4">
         <v>42138</v>
       </c>
@@ -1919,7 +1945,7 @@
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B108" s="4">
         <v>42139</v>
       </c>
@@ -1930,7 +1956,7 @@
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
     </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B109" s="5">
         <v>42140</v>
       </c>
@@ -1941,7 +1967,7 @@
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B110" s="5">
         <v>42141</v>
       </c>
@@ -1952,7 +1978,7 @@
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B111" s="4">
         <v>42142</v>
       </c>
@@ -1963,7 +1989,7 @@
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B112" s="4">
         <v>42143</v>
       </c>
@@ -1974,7 +2000,7 @@
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B113" s="4">
         <v>42144</v>
       </c>
@@ -1997,7 +2023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B114" s="4">
         <v>42145</v>
       </c>
@@ -2018,7 +2044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B115" s="4">
         <v>42146</v>
       </c>
@@ -2029,7 +2055,7 @@
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
     </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B116" s="5">
         <v>42147</v>
       </c>
@@ -2040,7 +2066,7 @@
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
     </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B117" s="5">
         <v>42148</v>
       </c>
@@ -2055,7 +2081,7 @@
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
     </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B118" s="4">
         <v>42149</v>
       </c>
@@ -2078,7 +2104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B119" s="4">
         <v>42150</v>
       </c>
@@ -2101,7 +2127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B120" s="4">
         <v>42151</v>
       </c>
@@ -2124,7 +2150,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B121" s="4">
         <v>42152</v>
       </c>
@@ -2135,7 +2161,7 @@
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
     </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B122" s="4">
         <v>42153</v>
       </c>
@@ -2146,7 +2172,7 @@
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
     </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B123" s="5">
         <v>42154</v>
       </c>
@@ -2167,7 +2193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B124" s="5">
         <v>42155</v>
       </c>
@@ -2182,11 +2208,11 @@
         <v>1.5</v>
       </c>
       <c r="G124" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H124" s="1"/>
     </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B125" s="4">
         <v>42156</v>
       </c>
@@ -2197,7 +2223,7 @@
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
     </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B126" s="4">
         <v>42157</v>
       </c>
@@ -2208,7 +2234,7 @@
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
     </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B127" s="4">
         <v>42158</v>
       </c>
@@ -2219,7 +2245,7 @@
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
     </row>
-    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B128" s="4">
         <v>42159</v>
       </c>
@@ -2230,7 +2256,7 @@
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
     </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B129" s="4">
         <v>42160</v>
       </c>
@@ -2253,7 +2279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B130" s="5">
         <v>42161</v>
       </c>
@@ -2276,7 +2302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B131" s="5">
         <v>42162</v>
       </c>
@@ -2299,7 +2325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B132" s="4">
         <v>42163</v>
       </c>
@@ -2320,7 +2346,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B133" s="4">
         <v>42164</v>
       </c>
@@ -2343,348 +2369,295 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B134" s="4">
+    <row r="134" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B134" s="15">
         <v>42165</v>
       </c>
-      <c r="C134" s="2"/>
-      <c r="D134" s="1"/>
-      <c r="E134" s="1"/>
-      <c r="F134" s="1"/>
-      <c r="G134" s="1"/>
-      <c r="H134" s="1"/>
-    </row>
-    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B135" s="4">
-        <v>42166</v>
-      </c>
-      <c r="C135" s="2"/>
-      <c r="D135" s="1"/>
-      <c r="E135" s="1"/>
-      <c r="F135" s="1"/>
-      <c r="G135" s="1"/>
-      <c r="H135" s="1"/>
-    </row>
-    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B136" s="4">
-        <v>42167</v>
-      </c>
-      <c r="C136" s="2"/>
-      <c r="D136" s="1"/>
-      <c r="E136" s="1"/>
-      <c r="F136" s="1"/>
-      <c r="G136" s="1"/>
-      <c r="H136" s="1"/>
-    </row>
-    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B137" s="5">
-        <v>42168</v>
-      </c>
-      <c r="C137" s="2"/>
-      <c r="D137" s="1"/>
-      <c r="E137" s="1"/>
-      <c r="F137" s="1"/>
-      <c r="G137" s="1"/>
-      <c r="H137" s="1"/>
-    </row>
-    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B138" s="5">
-        <v>42169</v>
-      </c>
-      <c r="C138" s="2"/>
-      <c r="D138" s="1"/>
-      <c r="E138" s="1"/>
-      <c r="F138" s="1"/>
-      <c r="G138" s="1"/>
-      <c r="H138" s="1"/>
-    </row>
-    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B139" s="4">
-        <v>42170</v>
-      </c>
-      <c r="C139" s="2"/>
-      <c r="D139" s="1"/>
-      <c r="E139" s="1"/>
-      <c r="F139" s="1"/>
-      <c r="G139" s="1"/>
-      <c r="H139" s="1"/>
-    </row>
-    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B140" s="4">
-        <v>42171</v>
-      </c>
-      <c r="C140" s="2"/>
-      <c r="D140" s="1"/>
-      <c r="E140" s="1"/>
-      <c r="F140" s="1"/>
-      <c r="G140" s="1"/>
-      <c r="H140" s="1"/>
-    </row>
-    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B141" s="4">
-        <v>42172</v>
-      </c>
-      <c r="C141" s="2"/>
-      <c r="D141" s="1"/>
-      <c r="E141" s="1"/>
-      <c r="F141" s="1"/>
-      <c r="G141" s="1"/>
-      <c r="H141" s="1"/>
-    </row>
-    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B142" s="4">
-        <v>42173</v>
-      </c>
-      <c r="C142" s="2"/>
-      <c r="D142" s="1"/>
-      <c r="E142" s="1"/>
-      <c r="F142" s="1"/>
-      <c r="G142" s="1"/>
-      <c r="H142" s="1"/>
-    </row>
-    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B143" s="4">
-        <v>42174</v>
-      </c>
-      <c r="C143" s="2"/>
-      <c r="D143" s="1"/>
-      <c r="E143" s="1"/>
-      <c r="F143" s="1"/>
-      <c r="G143" s="1"/>
-      <c r="H143" s="1"/>
-    </row>
-    <row r="144" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B144" s="5">
-        <v>42175</v>
-      </c>
-      <c r="C144" s="2"/>
-      <c r="D144" s="1"/>
-      <c r="E144" s="1"/>
-      <c r="F144" s="1"/>
-      <c r="G144" s="1"/>
-      <c r="H144" s="1"/>
-    </row>
-    <row r="145" spans="2:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B145" s="5">
-        <v>42176</v>
-      </c>
-      <c r="C145" s="2"/>
-      <c r="D145" s="1"/>
-      <c r="E145" s="1"/>
-      <c r="F145" s="1"/>
-      <c r="G145" s="1"/>
-      <c r="H145" s="1"/>
-    </row>
-    <row r="146" spans="2:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B146" s="4">
-        <v>42177</v>
-      </c>
-      <c r="C146" s="2"/>
-      <c r="D146" s="1"/>
-      <c r="E146" s="1"/>
-      <c r="F146" s="1"/>
-      <c r="G146" s="1"/>
-      <c r="H146" s="1"/>
-    </row>
-    <row r="147" spans="2:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B147" s="4">
-        <v>42178</v>
-      </c>
-      <c r="C147" s="2"/>
-      <c r="D147" s="1"/>
-      <c r="E147" s="1"/>
-      <c r="F147" s="1"/>
-      <c r="G147" s="1"/>
-      <c r="H147" s="1"/>
-    </row>
-    <row r="148" spans="2:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B148" s="4">
-        <v>42179</v>
-      </c>
-      <c r="C148" s="2"/>
-      <c r="D148" s="1"/>
-      <c r="E148" s="1"/>
-      <c r="F148" s="1"/>
-      <c r="G148" s="1"/>
-      <c r="H148" s="1"/>
-    </row>
-    <row r="149" spans="2:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B149" s="4">
-        <v>42180</v>
-      </c>
-      <c r="C149" s="2"/>
-      <c r="D149" s="1"/>
-      <c r="E149" s="1"/>
-      <c r="F149" s="1"/>
-      <c r="G149" s="1"/>
-      <c r="H149" s="1"/>
-    </row>
-    <row r="150" spans="2:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B150" s="4">
-        <v>42181</v>
-      </c>
-      <c r="C150" s="2"/>
-      <c r="D150" s="1"/>
-      <c r="E150" s="1"/>
-      <c r="F150" s="1"/>
-      <c r="G150" s="1"/>
-      <c r="H150" s="1"/>
-    </row>
-    <row r="151" spans="2:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B151" s="5">
-        <v>42182</v>
-      </c>
-      <c r="C151" s="2"/>
-      <c r="D151" s="2"/>
-      <c r="E151" s="2"/>
-      <c r="F151" s="2"/>
-      <c r="G151" s="2"/>
-      <c r="H151" s="2"/>
-    </row>
-    <row r="152" spans="2:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B152" s="5">
-        <v>42183</v>
-      </c>
-      <c r="C152" s="2"/>
-      <c r="D152" s="1"/>
-      <c r="E152" s="1"/>
-      <c r="F152" s="1"/>
-      <c r="G152" s="1"/>
-      <c r="H152" s="1"/>
-    </row>
-    <row r="153" spans="2:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B153" s="4">
-        <v>42184</v>
-      </c>
-      <c r="C153" s="2"/>
-      <c r="D153" s="1"/>
-      <c r="E153" s="1"/>
-      <c r="F153" s="1"/>
-      <c r="G153" s="1"/>
-      <c r="H153" s="1"/>
-    </row>
-    <row r="154" spans="2:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B154" s="4">
-        <v>42185</v>
-      </c>
-      <c r="C154" s="2"/>
-      <c r="D154" s="1"/>
-      <c r="E154" s="1"/>
-      <c r="F154" s="1"/>
-      <c r="G154" s="1"/>
-      <c r="H154" s="1"/>
-    </row>
-    <row r="155" spans="2:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B155" s="4">
-        <v>42186</v>
-      </c>
-      <c r="C155" s="2"/>
-      <c r="D155" s="1"/>
-      <c r="E155" s="1"/>
-      <c r="F155" s="1"/>
-      <c r="G155" s="1"/>
-      <c r="H155" s="1"/>
-    </row>
-    <row r="156" spans="2:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B156" s="4">
-        <v>42187</v>
-      </c>
-      <c r="C156" s="2"/>
-      <c r="D156" s="1"/>
-      <c r="E156" s="1"/>
-      <c r="F156" s="1"/>
-      <c r="G156" s="1"/>
-      <c r="H156" s="1"/>
-    </row>
-    <row r="157" spans="2:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B157" s="4">
-        <v>42188</v>
-      </c>
-      <c r="C157" s="2"/>
-      <c r="D157" s="1"/>
-      <c r="E157" s="1"/>
-      <c r="F157" s="1"/>
-      <c r="G157" s="1"/>
-      <c r="H157" s="1"/>
-    </row>
-    <row r="158" spans="2:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B158" s="5">
-        <v>42189</v>
-      </c>
-      <c r="C158" s="2"/>
-      <c r="D158" s="1"/>
-      <c r="E158" s="1"/>
-      <c r="F158" s="1"/>
-      <c r="G158" s="1"/>
-      <c r="H158" s="1"/>
-    </row>
-    <row r="159" spans="2:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B159" s="12">
-        <v>42190</v>
-      </c>
-      <c r="C159" s="13"/>
+      <c r="C134" s="12">
+        <v>4</v>
+      </c>
+      <c r="D134" s="13">
+        <v>4</v>
+      </c>
+      <c r="E134" s="13">
+        <v>4</v>
+      </c>
+      <c r="F134" s="13">
+        <v>4</v>
+      </c>
+      <c r="G134" s="13">
+        <v>4</v>
+      </c>
+      <c r="H134" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B135" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C135" s="24">
+        <f t="shared" ref="C135:H135" si="0">SUM(C6:C134)</f>
+        <v>79.5</v>
+      </c>
+      <c r="D135" s="22">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="E135" s="22">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="F135" s="22">
+        <f t="shared" si="0"/>
+        <v>84.5</v>
+      </c>
+      <c r="G135" s="22">
+        <f t="shared" si="0"/>
+        <v>60.5</v>
+      </c>
+      <c r="H135" s="23">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="I135" s="20">
+        <f>SUM(C135+D135+E135+F135+G135+G167)</f>
+        <v>375.5</v>
+      </c>
+    </row>
+    <row r="136" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B136" s="16"/>
+      <c r="C136" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D136" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E136" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F136" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G136" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H136" s="23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B137" s="19"/>
+      <c r="C137" s="14"/>
+      <c r="D137" s="14"/>
+      <c r="E137" s="14"/>
+      <c r="F137" s="14"/>
+      <c r="G137" s="14"/>
+      <c r="H137" s="14"/>
+    </row>
+    <row r="138" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B138" s="19"/>
+      <c r="C138" s="14"/>
+      <c r="D138" s="14"/>
+      <c r="E138" s="14"/>
+      <c r="F138" s="14"/>
+      <c r="G138" s="14"/>
+      <c r="H138" s="14"/>
+    </row>
+    <row r="139" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B139" s="16"/>
+      <c r="C139" s="14"/>
+      <c r="D139" s="14"/>
+      <c r="E139" s="14"/>
+      <c r="F139" s="14"/>
+      <c r="G139" s="14"/>
+      <c r="H139" s="14"/>
+    </row>
+    <row r="140" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B140" s="16"/>
+      <c r="C140" s="14"/>
+      <c r="D140" s="14"/>
+      <c r="E140" s="14"/>
+      <c r="F140" s="14"/>
+      <c r="G140" s="14"/>
+      <c r="H140" s="14"/>
+    </row>
+    <row r="141" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B141" s="16"/>
+      <c r="C141" s="14"/>
+      <c r="D141" s="14"/>
+      <c r="E141" s="14"/>
+      <c r="F141" s="14"/>
+      <c r="G141" s="14"/>
+      <c r="H141" s="14"/>
+    </row>
+    <row r="142" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B142" s="16"/>
+      <c r="C142" s="14"/>
+      <c r="D142" s="14"/>
+      <c r="E142" s="14"/>
+      <c r="F142" s="14"/>
+      <c r="G142" s="14"/>
+      <c r="H142" s="14"/>
+    </row>
+    <row r="143" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B143" s="19"/>
+      <c r="C143" s="14"/>
+      <c r="D143" s="14"/>
+      <c r="E143" s="14"/>
+      <c r="F143" s="14"/>
+      <c r="G143" s="14"/>
+      <c r="H143" s="14"/>
+    </row>
+    <row r="144" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C144" s="14"/>
+      <c r="D144" s="14"/>
+      <c r="E144" s="14"/>
+      <c r="F144" s="14"/>
+      <c r="G144" s="14"/>
+      <c r="H144" s="14"/>
+    </row>
+    <row r="145" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B145" s="19"/>
+      <c r="C145" s="14"/>
+      <c r="D145" s="14"/>
+      <c r="E145" s="14"/>
+      <c r="F145" s="14"/>
+      <c r="G145" s="14"/>
+      <c r="H145" s="14"/>
+    </row>
+    <row r="146" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B146" s="16"/>
+      <c r="C146" s="14"/>
+      <c r="D146" s="14"/>
+      <c r="E146" s="14"/>
+      <c r="F146" s="14"/>
+      <c r="G146" s="14"/>
+      <c r="H146" s="14"/>
+    </row>
+    <row r="147" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B147" s="16"/>
+      <c r="C147" s="14"/>
+      <c r="D147" s="14"/>
+      <c r="E147" s="14"/>
+      <c r="F147" s="14"/>
+      <c r="G147" s="14"/>
+      <c r="H147" s="14"/>
+    </row>
+    <row r="148" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B148" s="16"/>
+      <c r="C148" s="14"/>
+      <c r="D148" s="14"/>
+      <c r="E148" s="14"/>
+      <c r="F148" s="14"/>
+      <c r="G148" s="14"/>
+      <c r="H148" s="14"/>
+    </row>
+    <row r="149" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B149" s="16"/>
+      <c r="C149" s="14"/>
+      <c r="D149" s="14"/>
+      <c r="E149" s="14"/>
+      <c r="F149" s="14"/>
+      <c r="G149" s="14"/>
+      <c r="H149" s="14"/>
+    </row>
+    <row r="150" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B150" s="16"/>
+      <c r="C150" s="14"/>
+      <c r="D150" s="14"/>
+      <c r="E150" s="14"/>
+      <c r="F150" s="14"/>
+      <c r="G150" s="14"/>
+      <c r="H150" s="14"/>
+    </row>
+    <row r="151" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B151" s="19"/>
+      <c r="C151" s="14"/>
+      <c r="D151" s="14"/>
+      <c r="E151" s="14"/>
+      <c r="F151" s="14"/>
+      <c r="G151" s="14"/>
+      <c r="H151" s="14"/>
+    </row>
+    <row r="152" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B152" s="19"/>
+      <c r="C152" s="14"/>
+      <c r="D152" s="14"/>
+      <c r="E152" s="14"/>
+      <c r="F152" s="14"/>
+      <c r="G152" s="14"/>
+      <c r="H152" s="14"/>
+    </row>
+    <row r="153" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B153" s="16"/>
+      <c r="C153" s="14"/>
+      <c r="D153" s="14"/>
+      <c r="E153" s="14"/>
+      <c r="F153" s="14"/>
+      <c r="G153" s="14"/>
+      <c r="H153" s="14"/>
+    </row>
+    <row r="154" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B154" s="16"/>
+      <c r="C154" s="14"/>
+      <c r="D154" s="14"/>
+      <c r="E154" s="14"/>
+      <c r="F154" s="14"/>
+      <c r="G154" s="14"/>
+      <c r="H154" s="14"/>
+    </row>
+    <row r="155" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B155" s="16"/>
+      <c r="C155" s="14"/>
+      <c r="D155" s="14"/>
+      <c r="E155" s="14"/>
+      <c r="F155" s="14"/>
+      <c r="G155" s="14"/>
+      <c r="H155" s="14"/>
+    </row>
+    <row r="156" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B156" s="16"/>
+      <c r="C156" s="14"/>
+      <c r="D156" s="14"/>
+      <c r="E156" s="14"/>
+      <c r="F156" s="14"/>
+      <c r="G156" s="14"/>
+      <c r="H156" s="14"/>
+    </row>
+    <row r="157" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B157" s="16"/>
+      <c r="C157" s="14"/>
+      <c r="D157" s="14"/>
+      <c r="E157" s="14"/>
+      <c r="F157" s="14"/>
+      <c r="G157" s="14"/>
+      <c r="H157" s="14"/>
+    </row>
+    <row r="158" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B158" s="17"/>
+      <c r="C158" s="14"/>
+      <c r="D158" s="14"/>
+      <c r="E158" s="14"/>
+      <c r="F158" s="14"/>
+      <c r="G158" s="14"/>
+      <c r="H158" s="14"/>
+    </row>
+    <row r="159" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B159" s="17"/>
+      <c r="C159" s="14"/>
       <c r="D159" s="14"/>
       <c r="E159" s="14"/>
       <c r="F159" s="14"/>
       <c r="G159" s="14"/>
       <c r="H159" s="14"/>
     </row>
-    <row r="160" spans="2:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B160" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C160" s="17">
-        <f t="shared" ref="C160:H160" si="0">SUM(C6:C159)</f>
-        <v>75.5</v>
-      </c>
-      <c r="D160" s="10">
-        <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-      <c r="E160" s="10">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="F160" s="10">
-        <f t="shared" si="0"/>
-        <v>80.5</v>
-      </c>
-      <c r="G160" s="10">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="H160" s="15">
-        <f t="shared" si="0"/>
-        <v>55.5</v>
-      </c>
-      <c r="I160" s="8">
-        <f>SUM(C160+D160+E160+F160+G160+G167)</f>
-        <v>355</v>
-      </c>
-    </row>
-    <row r="161" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B161" s="16"/>
-      <c r="C161" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D161" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E161" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F161" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G161" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H161" s="11" t="s">
-        <v>5</v>
-      </c>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B161" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2694,7 +2667,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2706,7 +2679,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>